<commit_message>
Modified treatment column in 191031 data sheet as well as remaining jupyter notebooks
</commit_message>
<xml_diff>
--- a/191031_Deuterium_Transfer_Peak_Areas.xlsx
+++ b/191031_Deuterium_Transfer_Peak_Areas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Parker_research\GCMS_Stuff\191031\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF729BFA-6FE2-4160-9888-74D386E766F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DF0E607-1F5C-4C82-A571-C80DB49FF5F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19280" yWindow="760" windowWidth="19060" windowHeight="19730" xr2:uid="{0C4FD04D-EEC1-4A1F-94F8-64C84F3860BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,6 +32,15 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="25">
+  <si>
+    <t>#GCMS data for experiment recorded on 191029, accidentally flipped axis when extracting. Flipped WellNumber in this document. The well numbers in the GCMS files are wrong.</t>
+  </si>
+  <si>
+    <t>#Type refers to deuterium labelled ants (L) vs unlabelled ants (U)</t>
+  </si>
+  <si>
+    <t>#Outlier: Beetle or ant crushed/Beetle or ant escaped from well/Ant not coated in any CHCs (Y), Beetle chomped (B), ant chomped (A), normal run (N)</t>
+  </si>
   <si>
     <t>Species</t>
   </si>
@@ -69,10 +78,25 @@
     <t>A/H</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Outlier</t>
+  </si>
+  <si>
     <t>L</t>
   </si>
   <si>
     <t>C18</t>
+  </si>
+  <si>
+    <t>TIC</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
   <si>
     <t>D50C24</t>
@@ -81,38 +105,14 @@
     <t>D62C30</t>
   </si>
   <si>
-    <t>TIC</t>
-  </si>
-  <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>#Type refers to deuterium labelled ants (L) vs unlabelled ants (U)</t>
-  </si>
-  <si>
-    <t>#Outlier: Beetle or ant crushed/Beetle or ant escaped from well/Ant not coated in any CHCs (Y), Beetle chomped (B), ant chomped (A), normal run (N)</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Outlier</t>
-  </si>
-  <si>
-    <t>#GCMS data for experiment recorded on 191029, accidentally flipped axis when extracting. Flipped WellNumber in this document. The well numbers in the GCMS files are wrong.</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,80 +459,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9318726-D8BA-4845-AE33-2EE2376C2E04}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5:N52"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>7.431</v>
@@ -544,7 +544,7 @@
         <v>7.45</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H5">
         <v>2684324</v>
@@ -562,21 +562,21 @@
         <v>0.78</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D6">
         <v>9.48</v>
@@ -588,7 +588,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H6">
         <v>109</v>
@@ -606,21 +606,21 @@
         <v>2.27</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D7">
         <v>12.365</v>
@@ -632,7 +632,7 @@
         <v>12.365</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H7">
         <v>3456</v>
@@ -650,21 +650,21 @@
         <v>1.04</v>
       </c>
       <c r="M7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>17</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D8">
         <v>7.43</v>
@@ -676,7 +676,7 @@
         <v>7.45</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H8">
         <v>2841347</v>
@@ -694,21 +694,21 @@
         <v>0.76</v>
       </c>
       <c r="M8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>17</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D9">
         <v>9.5250000000000004</v>
@@ -720,7 +720,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H9">
         <v>1907</v>
@@ -738,21 +738,21 @@
         <v>1.5</v>
       </c>
       <c r="M9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>17</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>12.365</v>
@@ -764,7 +764,7 @@
         <v>12.365</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H10">
         <v>1789</v>
@@ -782,21 +782,21 @@
         <v>1.86</v>
       </c>
       <c r="M10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D11">
         <v>7.431</v>
@@ -808,7 +808,7 @@
         <v>7.45</v>
       </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H11">
         <v>3007496</v>
@@ -826,21 +826,21 @@
         <v>0.76</v>
       </c>
       <c r="M11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>9.4930000000000003</v>
@@ -852,7 +852,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H12">
         <v>188248</v>
@@ -870,21 +870,21 @@
         <v>1.02</v>
       </c>
       <c r="M12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D13">
         <v>12.343999999999999</v>
@@ -896,7 +896,7 @@
         <v>12.365</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H13">
         <v>392883</v>
@@ -914,21 +914,21 @@
         <v>1.77</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>17</v>
       </c>
       <c r="B14">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D14">
         <v>7.43</v>
@@ -940,7 +940,7 @@
         <v>7.45</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H14">
         <v>2970903</v>
@@ -958,21 +958,21 @@
         <v>0.76</v>
       </c>
       <c r="M14" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>17</v>
       </c>
       <c r="B15">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D15">
         <v>9.5250000000000004</v>
@@ -984,7 +984,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H15">
         <v>2967</v>
@@ -1002,21 +1002,21 @@
         <v>1.05</v>
       </c>
       <c r="M15" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>17</v>
       </c>
       <c r="B16">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D16">
         <v>12.365</v>
@@ -1028,7 +1028,7 @@
         <v>12.365</v>
       </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H16">
         <v>9396</v>
@@ -1046,21 +1046,21 @@
         <v>1.06</v>
       </c>
       <c r="M16" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D17">
         <v>7.43</v>
@@ -1072,7 +1072,7 @@
         <v>7.4550000000000001</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H17">
         <v>3226249</v>
@@ -1090,21 +1090,21 @@
         <v>0.77</v>
       </c>
       <c r="M17" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D18">
         <v>9.4920000000000009</v>
@@ -1116,7 +1116,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H18">
         <v>203235</v>
@@ -1134,21 +1134,21 @@
         <v>0.99</v>
       </c>
       <c r="M18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D19">
         <v>12.339</v>
@@ -1160,7 +1160,7 @@
         <v>12.365</v>
       </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H19">
         <v>159984</v>
@@ -1178,21 +1178,21 @@
         <v>1.75</v>
       </c>
       <c r="M19" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>17</v>
       </c>
       <c r="B20">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D20">
         <v>7.4290000000000003</v>
@@ -1204,7 +1204,7 @@
         <v>7.45</v>
       </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H20">
         <v>3218106</v>
@@ -1222,21 +1222,21 @@
         <v>0.79</v>
       </c>
       <c r="M20" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>17</v>
       </c>
       <c r="B21">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D21">
         <v>9.5250000000000004</v>
@@ -1248,7 +1248,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H21">
         <v>2083</v>
@@ -1266,21 +1266,21 @@
         <v>0.93</v>
       </c>
       <c r="M21" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>17</v>
       </c>
       <c r="B22">
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D22">
         <v>12.365</v>
@@ -1292,7 +1292,7 @@
         <v>12.365</v>
       </c>
       <c r="G22" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H22">
         <v>8879</v>
@@ -1310,21 +1310,21 @@
         <v>0.99</v>
       </c>
       <c r="M22" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D23">
         <v>7.43</v>
@@ -1336,7 +1336,7 @@
         <v>7.45</v>
       </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H23">
         <v>3252517</v>
@@ -1354,21 +1354,21 @@
         <v>0.76</v>
       </c>
       <c r="M23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B24">
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D24">
         <v>9.5250000000000004</v>
@@ -1380,7 +1380,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G24" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H24">
         <v>546</v>
@@ -1398,21 +1398,21 @@
         <v>2.59</v>
       </c>
       <c r="M24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B25">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D25">
         <v>12.365</v>
@@ -1424,7 +1424,7 @@
         <v>12.365</v>
       </c>
       <c r="G25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H25">
         <v>5968</v>
@@ -1442,21 +1442,21 @@
         <v>0.97</v>
       </c>
       <c r="M25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>17</v>
       </c>
       <c r="B26">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D26">
         <v>7.43</v>
@@ -1468,7 +1468,7 @@
         <v>7.4450000000000003</v>
       </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H26">
         <v>3162606</v>
@@ -1486,21 +1486,21 @@
         <v>0.76</v>
       </c>
       <c r="M26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>17</v>
       </c>
       <c r="B27">
         <v>5</v>
       </c>
       <c r="C27" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D27">
         <v>9.5250000000000004</v>
@@ -1512,7 +1512,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H27">
         <v>2685</v>
@@ -1530,21 +1530,21 @@
         <v>1.06</v>
       </c>
       <c r="M27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>17</v>
       </c>
       <c r="B28">
         <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D28">
         <v>12.365</v>
@@ -1556,7 +1556,7 @@
         <v>12.365</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H28">
         <v>5686</v>
@@ -1574,21 +1574,21 @@
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B29">
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D29">
         <v>7.43</v>
@@ -1600,7 +1600,7 @@
         <v>7.45</v>
       </c>
       <c r="G29" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H29">
         <v>3218719</v>
@@ -1618,21 +1618,21 @@
         <v>0.76</v>
       </c>
       <c r="M29" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B30">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D30">
         <v>9.4930000000000003</v>
@@ -1644,7 +1644,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G30" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H30">
         <v>135511</v>
@@ -1662,21 +1662,21 @@
         <v>1.03</v>
       </c>
       <c r="M30" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B31">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D31">
         <v>12.340999999999999</v>
@@ -1688,7 +1688,7 @@
         <v>12.365</v>
       </c>
       <c r="G31" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H31">
         <v>419316</v>
@@ -1706,21 +1706,21 @@
         <v>1.83</v>
       </c>
       <c r="M31" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>17</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D32">
         <v>7.4290000000000003</v>
@@ -1732,7 +1732,7 @@
         <v>7.45</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H32">
         <v>3186253</v>
@@ -1750,21 +1750,21 @@
         <v>0.75</v>
       </c>
       <c r="M32" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>17</v>
       </c>
       <c r="B33">
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D33">
         <v>9.5250000000000004</v>
@@ -1776,7 +1776,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G33" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H33">
         <v>2408</v>
@@ -1794,21 +1794,21 @@
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>17</v>
       </c>
       <c r="B34">
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D34">
         <v>12.365</v>
@@ -1820,7 +1820,7 @@
         <v>12.365</v>
       </c>
       <c r="G34" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H34">
         <v>7064</v>
@@ -1838,21 +1838,21 @@
         <v>0.99</v>
       </c>
       <c r="M34" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B35">
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D35">
         <v>7.43</v>
@@ -1864,7 +1864,7 @@
         <v>7.45</v>
       </c>
       <c r="G35" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H35">
         <v>3156149</v>
@@ -1882,21 +1882,21 @@
         <v>0.78</v>
       </c>
       <c r="M35" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D36">
         <v>9.5250000000000004</v>
@@ -1908,7 +1908,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H36">
         <v>45</v>
@@ -1926,21 +1926,21 @@
         <v>0.98</v>
       </c>
       <c r="M36" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B37">
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D37">
         <v>12.365</v>
@@ -1952,7 +1952,7 @@
         <v>12.365</v>
       </c>
       <c r="G37" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H37">
         <v>4612</v>
@@ -1970,21 +1970,21 @@
         <v>0.91</v>
       </c>
       <c r="M37" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>17</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D38">
         <v>7.4279999999999999</v>
@@ -1996,7 +1996,7 @@
         <v>7.4649999999999999</v>
       </c>
       <c r="G38" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H38">
         <v>3178716</v>
@@ -2014,21 +2014,21 @@
         <v>0.8</v>
       </c>
       <c r="M38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>17</v>
       </c>
       <c r="B39">
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D39">
         <v>9.5250000000000004</v>
@@ -2040,7 +2040,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G39" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H39">
         <v>3110</v>
@@ -2058,21 +2058,21 @@
         <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>17</v>
       </c>
       <c r="B40">
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D40">
         <v>12.365</v>
@@ -2084,7 +2084,7 @@
         <v>12.365</v>
       </c>
       <c r="G40" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H40">
         <v>4894</v>
@@ -2102,21 +2102,21 @@
         <v>1.03</v>
       </c>
       <c r="M40" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D41">
         <v>7.4279999999999999</v>
@@ -2128,7 +2128,7 @@
         <v>7.4550000000000001</v>
       </c>
       <c r="G41" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H41">
         <v>3158755</v>
@@ -2146,21 +2146,21 @@
         <v>0.8</v>
       </c>
       <c r="M41" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D42">
         <v>9.5220000000000002</v>
@@ -2172,7 +2172,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G42" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H42">
         <v>118</v>
@@ -2190,21 +2190,21 @@
         <v>2.23</v>
       </c>
       <c r="M42" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B43">
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D43">
         <v>12.365</v>
@@ -2216,7 +2216,7 @@
         <v>12.365</v>
       </c>
       <c r="G43" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H43">
         <v>6259</v>
@@ -2234,21 +2234,21 @@
         <v>0.95</v>
       </c>
       <c r="M43" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>17</v>
       </c>
       <c r="B44">
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D44">
         <v>7.4279999999999999</v>
@@ -2260,7 +2260,7 @@
         <v>7.45</v>
       </c>
       <c r="G44" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H44">
         <v>3077419</v>
@@ -2278,21 +2278,21 @@
         <v>0.78</v>
       </c>
       <c r="M44" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N44" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>17</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D45">
         <v>9.4969999999999999</v>
@@ -2304,7 +2304,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G45" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H45">
         <v>7292</v>
@@ -2322,21 +2322,21 @@
         <v>1.99</v>
       </c>
       <c r="M45" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N45" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>17</v>
       </c>
       <c r="B46">
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D46">
         <v>12.365</v>
@@ -2348,7 +2348,7 @@
         <v>12.365</v>
       </c>
       <c r="G46" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H46">
         <v>7503</v>
@@ -2366,21 +2366,21 @@
         <v>1.22</v>
       </c>
       <c r="M46" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D47">
         <v>7.4279999999999999</v>
@@ -2392,7 +2392,7 @@
         <v>7.45</v>
       </c>
       <c r="G47" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H47">
         <v>3565793</v>
@@ -2410,21 +2410,21 @@
         <v>0.86</v>
       </c>
       <c r="M47" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N47" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D48">
         <v>9.4909999999999997</v>
@@ -2436,7 +2436,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G48" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H48">
         <v>105983</v>
@@ -2454,21 +2454,21 @@
         <v>0.97</v>
       </c>
       <c r="M48" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N48" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D49">
         <v>12.336</v>
@@ -2480,7 +2480,7 @@
         <v>12.365</v>
       </c>
       <c r="G49" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H49">
         <v>179711</v>
@@ -2498,21 +2498,21 @@
         <v>1.8</v>
       </c>
       <c r="M49" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>17</v>
       </c>
       <c r="B50">
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D50">
         <v>7.4279999999999999</v>
@@ -2524,7 +2524,7 @@
         <v>7.45</v>
       </c>
       <c r="G50" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H50">
         <v>3218004</v>
@@ -2542,21 +2542,21 @@
         <v>0.8</v>
       </c>
       <c r="M50" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>17</v>
       </c>
       <c r="B51">
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="D51">
         <v>9.4960000000000004</v>
@@ -2568,7 +2568,7 @@
         <v>9.5250000000000004</v>
       </c>
       <c r="G51" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H51">
         <v>10254</v>
@@ -2586,21 +2586,21 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="M51" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>17</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D52">
         <v>12.365</v>
@@ -2612,7 +2612,7 @@
         <v>12.365</v>
       </c>
       <c r="G52" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H52">
         <v>13626</v>
@@ -2630,10 +2630,10 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="M52" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="N52" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>